<commit_message>
update full m/s data, figs
</commit_message>
<xml_diff>
--- a/Data/Datatables_ms.xlsx
+++ b/Data/Datatables_ms.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristakraskura/Github_repositories/KK_etal_gobies_tempVar_tempTol/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980B2736-1DB9-844A-BBA5-9EFA76E86B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5982852F-D385-8E4D-97A6-864746A31DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="500" windowWidth="23220" windowHeight="15700" xr2:uid="{C7FD16A5-6D6F-ED42-9CEB-C21D96802EB4}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="23220" windowHeight="15700" xr2:uid="{C7FD16A5-6D6F-ED42-9CEB-C21D96802EB4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Figure 1 C" sheetId="1" r:id="rId1"/>
+    <sheet name="In text values" sheetId="3" r:id="rId2"/>
+    <sheet name="Suppl Table 1" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
   <si>
     <t>SITE1</t>
   </si>
@@ -66,13 +68,70 @@
   </si>
   <si>
     <t>Site Specific means and maxes, Table 1</t>
+  </si>
+  <si>
+    <t>±</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Daily Min (mean +/- SD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily Max </t>
+  </si>
+  <si>
+    <t>(mean +/- SD)</t>
+  </si>
+  <si>
+    <t>Daily Mean (mean +/- SD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily ∆ </t>
+  </si>
+  <si>
+    <t>Recording time span</t>
+  </si>
+  <si>
+    <t>Site 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-09-17 to 2021-07-05 </t>
+  </si>
+  <si>
+    <t>Site 2</t>
+  </si>
+  <si>
+    <t>2019-09-17 to 2019-09-26</t>
+  </si>
+  <si>
+    <t>Site 3</t>
+  </si>
+  <si>
+    <t>2019-09-26 to 2021-07-05</t>
+  </si>
+  <si>
+    <t>Site 4</t>
+  </si>
+  <si>
+    <t>2019-09-17 to 2020-02-02</t>
+  </si>
+  <si>
+    <t>Test Site</t>
+  </si>
+  <si>
+    <t>2021-07-06 to 2022-04-11</t>
+  </si>
+  <si>
+    <t>n (days)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +147,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -97,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -105,11 +170,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -117,6 +262,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,30 +610,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2699860-745F-E14A-AEFD-805F79CD608E}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:F28"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" s="2"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+    </row>
+    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -465,18 +658,42 @@
       <c r="C3">
         <v>11.1</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
         <v>4.7</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>658</v>
       </c>
-      <c r="F3" s="3" t="str">
-        <f>CONCATENATE(C3, " +/- ", D3)</f>
-        <v>11.1 +/- 4.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="3" t="str">
+        <f>CONCATENATE(C3, " ",D3," ", E3)</f>
+        <v>11.1 ± 4.7</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -486,18 +703,32 @@
       <c r="C4">
         <v>15.2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
         <v>1.54</v>
       </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3" t="str">
-        <f t="shared" ref="F4:F7" si="0">CONCATENATE(C4, " +/- ", D4)</f>
-        <v>15.2 +/- 1.54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="str">
+        <f t="shared" ref="G4:G7" si="0">CONCATENATE(C4, " ",D4," ", E4)</f>
+        <v>15.2 ± 1.54</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="16"/>
+      <c r="M4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="16"/>
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -507,18 +738,46 @@
       <c r="C5">
         <v>13.5</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
         <v>3.87</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>649</v>
       </c>
-      <c r="F5" s="3" t="str">
+      <c r="G5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>13.5 +/- 3.87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13.5 ± 3.87</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="5" t="str">
+        <f>G3</f>
+        <v>11.1 ± 4.7</v>
+      </c>
+      <c r="K5" s="5" t="str">
+        <f>G10</f>
+        <v>26.1 ± 5.33</v>
+      </c>
+      <c r="L5" s="5" t="str">
+        <f>G17</f>
+        <v>17 ± 4.36</v>
+      </c>
+      <c r="M5" s="5" t="str">
+        <f>G24</f>
+        <v>15 ± 4.06</v>
+      </c>
+      <c r="N5" s="5">
+        <v>93565</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -528,18 +787,46 @@
       <c r="C6">
         <v>13.3</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
         <v>2.79</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>139</v>
       </c>
-      <c r="F6" s="3" t="str">
+      <c r="G6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>13.3 +/- 2.79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13.3 ± 2.79</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="5" t="str">
+        <f>G4</f>
+        <v>15.2 ± 1.54</v>
+      </c>
+      <c r="K6" s="5" t="str">
+        <f t="shared" ref="K6:K9" si="1">G11</f>
+        <v>28.6 ± 2.71</v>
+      </c>
+      <c r="L6" s="5" t="str">
+        <f t="shared" ref="L6:L9" si="2">G18</f>
+        <v>21.2 ± 1.75</v>
+      </c>
+      <c r="M6" s="5" t="str">
+        <f t="shared" ref="M6:M9" si="3">G25</f>
+        <v>13.4 ± 2.48</v>
+      </c>
+      <c r="N6" s="5">
+        <v>1114</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -549,23 +836,107 @@
       <c r="C7">
         <v>14.6</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7">
         <v>3.15</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>280</v>
       </c>
-      <c r="F7" s="3" t="str">
+      <c r="G7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>14.6 +/- 3.15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14.6 ± 3.15</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="5" t="str">
+        <f t="shared" ref="J7:J9" si="4">G5</f>
+        <v>13.5 ± 3.87</v>
+      </c>
+      <c r="K7" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>24.1 ± 5.74</v>
+      </c>
+      <c r="L7" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>17.8 ± 3.73</v>
+      </c>
+      <c r="M7" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>10.6 ± 4.14</v>
+      </c>
+      <c r="N7" s="5">
+        <v>93216</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D8" s="4"/>
+      <c r="G8" s="3"/>
+      <c r="I8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>13.3 ± 2.79</v>
+      </c>
+      <c r="K8" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>19.4 ± 3.38</v>
+      </c>
+      <c r="L8" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>16.3 ± 2.6</v>
+      </c>
+      <c r="M8" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>6.03 ± 1.8</v>
+      </c>
+      <c r="N8" s="5">
+        <v>19907</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D9" s="4"/>
+      <c r="G9" s="3"/>
+      <c r="I9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>14.6 ± 3.15</v>
+      </c>
+      <c r="K9" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>20.3 ± 4.28</v>
+      </c>
+      <c r="L9" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>17.1 ± 3.15</v>
+      </c>
+      <c r="M9" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>5.74 ± 2.05</v>
+      </c>
+      <c r="N9" s="9">
+        <v>30565</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -575,18 +946,21 @@
       <c r="C10">
         <v>26.1</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10">
         <v>5.33</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>658</v>
       </c>
-      <c r="F10" s="3" t="str">
-        <f>CONCATENATE(C10, " +/- ", D10)</f>
-        <v>26.1 +/- 5.33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="3" t="str">
+        <f>CONCATENATE(C10, " ",D10," ", E10)</f>
+        <v>26.1 ± 5.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -596,18 +970,21 @@
       <c r="C11">
         <v>28.6</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11">
         <v>2.71</v>
       </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3" t="str">
-        <f t="shared" ref="F11:F14" si="1">CONCATENATE(C11, " +/- ", D11)</f>
-        <v>28.6 +/- 2.71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" s="3" t="str">
+        <f t="shared" ref="G11:G14" si="5">CONCATENATE(C11, " ",D11," ", E11)</f>
+        <v>28.6 ± 2.71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3</v>
       </c>
@@ -617,18 +994,21 @@
       <c r="C12">
         <v>24.1</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12">
         <v>5.74</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>649</v>
       </c>
-      <c r="F12" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>24.1 +/- 5.74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>24.1 ± 5.74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -638,18 +1018,21 @@
       <c r="C13">
         <v>19.399999999999999</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13">
         <v>3.38</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>139</v>
       </c>
-      <c r="F13" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>19.4 +/- 3.38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>19.4 ± 3.38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -659,23 +1042,32 @@
       <c r="C14">
         <v>20.3</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14">
         <v>4.28</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>280</v>
       </c>
-      <c r="F14" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>20.3 +/- 4.28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>20.3 ± 4.28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D15" s="4"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D16" s="4"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -685,18 +1077,21 @@
       <c r="C17">
         <v>17</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17">
         <v>4.3600000000000003</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>658</v>
       </c>
-      <c r="F17" s="3" t="str">
-        <f>CONCATENATE(C17, " +/- ", D17)</f>
-        <v>17 +/- 4.36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="3" t="str">
+        <f>CONCATENATE(C17, " ",D17," ", E17)</f>
+        <v>17 ± 4.36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -706,18 +1101,21 @@
       <c r="C18">
         <v>21.2</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18">
         <v>1.75</v>
       </c>
-      <c r="E18">
-        <v>10</v>
-      </c>
-      <c r="F18" s="3" t="str">
-        <f t="shared" ref="F18:F21" si="2">CONCATENATE(C18, " +/- ", D18)</f>
-        <v>21.2 +/- 1.75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18" s="3" t="str">
+        <f t="shared" ref="G18:G21" si="6">CONCATENATE(C18, " ",D18," ", E18)</f>
+        <v>21.2 ± 1.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -727,18 +1125,21 @@
       <c r="C19">
         <v>17.8</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19">
         <v>3.73</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>649</v>
       </c>
-      <c r="F19" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>17.8 +/- 3.73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>17.8 ± 3.73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4</v>
       </c>
@@ -748,18 +1149,21 @@
       <c r="C20">
         <v>16.3</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20">
         <v>2.6</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>139</v>
       </c>
-      <c r="F20" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>16.3 +/- 2.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>16.3 ± 2.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>5</v>
       </c>
@@ -769,23 +1173,32 @@
       <c r="C21">
         <v>17.100000000000001</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21">
         <v>3.15</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>280</v>
       </c>
-      <c r="F21" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>17.1 +/- 3.15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>17.1 ± 3.15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D22" s="4"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D23" s="4"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -795,18 +1208,21 @@
       <c r="C24">
         <v>15</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24">
         <v>4.0599999999999996</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>658</v>
       </c>
-      <c r="F24" s="3" t="str">
-        <f>CONCATENATE(C24, " +/- ", D24)</f>
-        <v>15 +/- 4.06</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="3" t="str">
+        <f>CONCATENATE(C24, " ",D24," ", E24)</f>
+        <v>15 ± 4.06</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -816,18 +1232,21 @@
       <c r="C25">
         <v>13.4</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25">
         <v>2.48</v>
       </c>
-      <c r="E25">
-        <v>10</v>
-      </c>
-      <c r="F25" s="3" t="str">
-        <f t="shared" ref="F25:F28" si="3">CONCATENATE(C25, " +/- ", D25)</f>
-        <v>13.4 +/- 2.48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="G25" s="3" t="str">
+        <f t="shared" ref="G25:G28" si="7">CONCATENATE(C25, " ",D25," ", E25)</f>
+        <v>13.4 ± 2.48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -837,18 +1256,21 @@
       <c r="C26">
         <v>10.6</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26">
         <v>4.1399999999999997</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>649</v>
       </c>
-      <c r="F26" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>10.6 +/- 4.14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>10.6 ± 4.14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -858,18 +1280,21 @@
       <c r="C27">
         <v>6.03</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27">
         <v>1.8</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>139</v>
       </c>
-      <c r="F27" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>6.03 +/- 1.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>6.03 ± 1.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>5</v>
       </c>
@@ -879,18 +1304,56 @@
       <c r="C28">
         <v>5.74</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28">
         <v>2.0499999999999998</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>280</v>
       </c>
-      <c r="F28" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>5.74 +/- 2.05</v>
+      <c r="G28" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>5.74 ± 2.05</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1142CAA0-8D4A-9B4F-A595-47983E645F1F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6B25FA-E12C-9342-968B-84F8C5E44A66}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>